<commit_message>
#Nhập kho - Bổ sung ngày sx/hh
</commit_message>
<xml_diff>
--- a/Document/2.Design/Template/Bieu_mau_nhap_hang.xlsx
+++ b/Document/2.Design/Template/Bieu_mau_nhap_hang.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WMS\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\WMS\WMS\Document\2.Design\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9518B50E-919B-44FE-B4E6-439A07AF49DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tên hàng</t>
   </si>
@@ -45,7 +46,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -61,7 +62,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -77,7 +78,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -93,7 +94,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -103,25 +104,64 @@
 2: Hỏng</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngày sản xuất 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(dd/MM/yyyy)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngày hết hạn
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(dd/MM/yyyy)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -487,26 +527,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="2" max="2" width="22.125" customWidth="1"/>
-    <col min="3" max="3" width="39.375" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="28.75" customWidth="1"/>
-    <col min="6" max="6" width="11.375" customWidth="1"/>
-    <col min="7" max="7" width="17.75" customWidth="1"/>
-    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -530,6 +572,12 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>